<commit_message>
meest recente Excel Template
</commit_message>
<xml_diff>
--- a/OnePage/src/Excel/OnePageTemplate.xlsx
+++ b/OnePage/src/Excel/OnePageTemplate.xlsx
@@ -11,6 +11,58 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Luinenburg, Mendelt</author>
+  </authors>
+  <commentList>
+    <comment ref="A17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Schrijf hier wat over jezelf</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vul hier een waarde tussen 0(junior) en 100(senior) in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LinkedIn URL kan je via je profiel verkorten.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
@@ -123,9 +175,6 @@
     <t>Hoogste opleiding</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Situatie:</t>
   </si>
   <si>
@@ -138,14 +187,17 @@
     <t>Skills/Vaardigheden</t>
   </si>
   <si>
-    <t>Beste collega, leuk dat je gebruik wil maken van de Ordina One Page generator. De tool is op dit moment nog vol in ontwikkeling, dus alle feedback is welkom.                                                                    Gebruiksaanwijzing: vul alle lichter getinte velden in met de juiste persoonsinformatie. De grootte van de textvelden is een benadering van de grootte van textvelden op het eindproduct, dus probeer erbinnen te blijven. Zodra je klaar bent, exporteer de gegevens naar [Naam].xml, waar je je naam invult zoals op dit formulier. Lever ook een pasfoto met dezelfde naam aan.</t>
+    <t>Beste collega, leuk dat je gebruik wil maken van de Ordina One Page generator. De tool is op dit moment nog vol in ontwikkeling, dus alle feedback is welkom.                                                                    Gebruiksaanwijzing: vul alle lichter getinte velden in met de juiste persoonsinformatie. De grootte van de textvelden is een benadering van de grootte van textvelden op het eindproduct, dus probeer erbinnen te blijven. Zodra je klaar bent, exporteer de gegevens naar [Naam].xml, waar je je naam invult zoals op dit formulier. Lever ook een vierkante pasfoto met dezelfde naam aan.</t>
+  </si>
+  <si>
+    <t>contact: mendelt.luinenburg@ordina.nl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +251,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -274,6 +333,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -283,10 +346,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1087,11 +1146,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,22 +1166,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="17"/>
       <c r="D2" s="7" t="s">
@@ -1154,9 +1213,9 @@
       </c>
       <c r="E4" s="8"/>
       <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
@@ -1166,7 +1225,7 @@
       </c>
       <c r="E5" s="8"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="12"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
@@ -1176,7 +1235,7 @@
       </c>
       <c r="E6" s="8"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
@@ -1186,7 +1245,7 @@
       </c>
       <c r="E7" s="8"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
@@ -1196,7 +1255,7 @@
       </c>
       <c r="E8" s="8"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="12"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
@@ -1206,7 +1265,7 @@
       </c>
       <c r="E9" s="8"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
@@ -1216,9 +1275,9 @@
       </c>
       <c r="E10" s="8"/>
       <c r="G10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
@@ -1228,7 +1287,7 @@
       </c>
       <c r="E11" s="8"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
@@ -1238,7 +1297,7 @@
       </c>
       <c r="E12" s="8"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
@@ -1248,7 +1307,7 @@
       </c>
       <c r="E13" s="8"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -1258,7 +1317,7 @@
       </c>
       <c r="E14" s="8"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1270,7 +1329,7 @@
       </c>
       <c r="E15" s="8"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1282,59 +1341,59 @@
       </c>
       <c r="E16" s="8"/>
       <c r="G16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="15"/>
       <c r="D17" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="8"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="11"/>
+      <c r="B18" s="15"/>
       <c r="D18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="8"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="11"/>
+      <c r="B19" s="15"/>
       <c r="D19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="8"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="12"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="11"/>
+      <c r="B20" s="15"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="15"/>
       <c r="D21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="11"/>
+      <c r="B22" s="15"/>
       <c r="D22" s="4" t="s">
         <v>18</v>
       </c>
@@ -1346,7 +1405,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="11"/>
+      <c r="B23" s="15"/>
       <c r="D23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1358,7 +1417,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="11"/>
+      <c r="B24" s="15"/>
       <c r="D24" s="4" t="s">
         <v>21</v>
       </c>
@@ -1370,7 +1429,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="15"/>
       <c r="D25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1378,27 +1437,27 @@
       <c r="G25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="10"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="11"/>
+      <c r="B26" s="15"/>
       <c r="D26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="2"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="10"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="11"/>
+      <c r="B27" s="15"/>
       <c r="D27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="2"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="10"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
@@ -1436,7 +1495,7 @@
       <c r="G30" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="10"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -1448,7 +1507,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="10"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -1460,7 +1519,7 @@
       </c>
       <c r="E32" s="2"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="10"/>
+      <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -1498,7 +1557,7 @@
       <c r="G35" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="10"/>
+      <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
@@ -1506,7 +1565,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="10"/>
+      <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
@@ -1514,24 +1573,24 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="10"/>
+      <c r="H37" s="14"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
-        <v>30</v>
+      <c r="A39" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
+      <c r="A40" s="10"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
+      <c r="A41" s="10"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
+      <c r="A42" s="10"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
+      <c r="A43" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1546,5 +1605,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>